<commit_message>
files updated and bug fixed
</commit_message>
<xml_diff>
--- a/municipal/ENG/Education/Preschool and Education Institutions/Adjara A.R/Khulo.xlsx
+++ b/municipal/ENG/Education/Preschool and Education Institutions/Adjara A.R/Khulo.xlsx
@@ -269,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,6 +329,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -342,14 +351,17 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,7 +646,7 @@
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="D5" sqref="D5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,16 +660,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -667,16 +679,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -714,11 +726,11 @@
       <c r="R3" s="21"/>
     </row>
     <row r="4" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="9">
         <v>20</v>
       </c>
@@ -746,25 +758,25 @@
       <c r="R4" s="21"/>
     </row>
     <row r="5" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="12">
-        <v>25.972495088408643</v>
-      </c>
-      <c r="E5" s="13">
-        <v>23.897768512084006</v>
-      </c>
-      <c r="F5" s="14">
-        <v>24.754360575824506</v>
-      </c>
-      <c r="G5" s="13">
-        <v>24.675129572598209</v>
-      </c>
-      <c r="H5" s="13">
-        <v>22.955951404934037</v>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="30">
+        <v>661</v>
+      </c>
+      <c r="E5" s="31">
+        <v>619</v>
+      </c>
+      <c r="F5" s="32">
+        <v>650</v>
+      </c>
+      <c r="G5" s="31">
+        <v>657</v>
+      </c>
+      <c r="H5" s="33">
+        <v>616</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -778,11 +790,11 @@
       <c r="R5" s="21"/>
     </row>
     <row r="6" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="15">
         <v>66</v>
       </c>
@@ -810,11 +822,11 @@
       <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="12">
         <v>10.015151515151516</v>
       </c>
@@ -852,11 +864,11 @@
       <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="14">
         <v>25.972495088408643</v>
       </c>
@@ -894,11 +906,11 @@
       <c r="AB8" s="1"/>
     </row>
     <row r="9" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="20">
         <v>1272.5000000000002</v>
       </c>
@@ -923,10 +935,10 @@
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="28"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -938,11 +950,11 @@
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -966,16 +978,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:E11"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>